<commit_message>
Glossary QA for KMS控制台中文.xlsx
</commit_message>
<xml_diff>
--- a/console/Cloud-Security/KMS控制台中文.xlsx
+++ b/console/Cloud-Security/KMS控制台中文.xlsx
@@ -88,10 +88,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>自定义</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -638,10 +634,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Key List</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Create</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -650,10 +642,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Key Status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Creation Time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -666,10 +654,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Copy Successfully</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Enabled</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -702,30 +686,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>No Key Data Available</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Purpose Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Is alternating Required or Not</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Alternating Period</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Customized</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Are you sure to enable the selected key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -734,10 +702,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Are you sure to disable the selected key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Plan to Delete Time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -758,10 +722,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Please enter the key name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>The name cannot exceed 32 characters</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -790,42 +750,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Create new key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Notification</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Enable the key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Disable the key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Plan to delete key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Key Information</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Key Detail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Online Tool</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Key Details</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Modify Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -834,10 +770,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Key ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Purpose Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -886,10 +818,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>The name cannot be blank</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>The length cannot be more than 4,096 characters</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -906,14 +834,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Key Version</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Main Key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>No Alternating Data Available</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -922,10 +842,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Are you sure to create new version key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Are you sure to cancel deletion operation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1054,14 +970,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Are you sure to delete these n keys</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Have selected n keys</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>n cannot be enabled</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1090,14 +998,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Key ID error, please check</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Key name error, please check</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Confidential ID error, please check</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1110,10 +1010,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Key alternating cycle error, please check</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Date error, please check</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1130,10 +1026,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Key already exists, please check and then try again</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Name exceeds the maximum length, submit after modification</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1150,10 +1042,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>The quantity of keys has reached the cap</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>The quantity of secrets has reached the cap</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1189,14 +1077,6 @@
     <t>Service enabling failed. Please try again</t>
   </si>
   <si>
-    <t>Key Management Service</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KMS key management service is used as security management service product. By means of key management service, you can use the key securely and conveniently, and focus on the decryption function scenario and application required by business</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Key management service has the following functions and advantages</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1229,15 +1109,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Support over-the-cloud OSS object storage, elastic block storage (EBS), RDS relational database encryption, convenient to integrate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Security and Reliability</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Key is protected by HSM hardware module, to key the key secure and reliable</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1264,6 +1136,134 @@
       </rPr>
       <t>译文</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key Pair List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Copied</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No Key Pair Data Available</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you sure to enable the selected key pair </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you sure to disable the selected key pair </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Please enter the key pair name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Create new key pair </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable the key pair </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Disable the key pair </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan to delete key pair </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key Pair Detail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key Pair Details</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key Pair ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Must provide a name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key Pair Version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Main Key Pair </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Are you sure to create new version key pair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Are you sure to delete these n key pairs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Have selected n key pairs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key Pair ID error, please check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key pair name error, please check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key pair alternating cycle error, please check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key pair already exists, please check and then try again</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The quantity of key pairs has reached the cap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key Pair Management Service</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KMS key pair management service is used as security management service product. By means of key management service, you can use the key pair securely and conveniently, and focus on the decryption function scenario and application required by business</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Support over-the-cloud OSS, elastic block storage (EBS), RDS relational database encryption, convenient to integrate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key pair is protected by HSM hardware module, to key the key secure and reliable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key Pair Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is alternating required or not</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Customized</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自定义</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1360,10 +1360,18 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1646,1247 +1654,1247 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="74.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="74.875" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.625" style="1"/>
+    <col min="1" max="1" width="29.75" style="3" customWidth="1"/>
+    <col min="2" max="2" width="68.625" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="13.5">
+      <c r="A1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="3" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="B22" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="4" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="4" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="4" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="4" t="s">
+    <row r="29" spans="1:2">
+      <c r="A29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="4" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="4" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B23" s="4" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="4" t="s">
+    <row r="34" spans="1:2" ht="28.5">
+      <c r="A34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="4" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B26" s="4" t="s">
+    <row r="36" spans="1:2">
+      <c r="A36" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="4" t="s">
+    <row r="37" spans="1:2">
+      <c r="A37" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="4" t="s">
+    <row r="38" spans="1:2">
+      <c r="A38" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="4" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="4" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="4" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="4" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="4" t="s">
+    <row r="48" spans="1:2">
+      <c r="A48" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="4" t="s">
+    <row r="50" spans="1:2">
+      <c r="A50" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="4" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" s="4" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" s="3" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B37" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="4" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" s="4" t="s">
+    <row r="55" spans="1:2">
+      <c r="A55" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="4" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" s="4" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="4" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="4" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="4" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" s="4" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B46" s="4" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B47" s="4" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="4" t="s">
+    <row r="65" spans="1:2">
+      <c r="A65" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B49" s="4" t="s">
+    <row r="66" spans="1:2" ht="41.25">
+      <c r="A66" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B50" s="4" t="s">
+    <row r="67" spans="1:2">
+      <c r="A67" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B67" s="4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51" s="4" t="s">
+    <row r="68" spans="1:2">
+      <c r="A68" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B52" s="4" t="s">
+    <row r="71" spans="1:2">
+      <c r="A71" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="1" t="s">
+    <row r="72" spans="1:2">
+      <c r="A72" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B53" s="4" t="s">
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B54" s="4" t="s">
+    <row r="75" spans="1:2">
+      <c r="A75" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B55" s="4" t="s">
+    <row r="76" spans="1:2">
+      <c r="A76" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B56" s="4" t="s">
+    <row r="77" spans="1:2">
+      <c r="A77" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77" s="4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B57" s="4" t="s">
+    <row r="78" spans="1:2">
+      <c r="A78" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B78" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B58" s="4" t="s">
+    <row r="79" spans="1:2">
+      <c r="A79" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B79" s="4" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B59" s="4" t="s">
+    <row r="80" spans="1:2">
+      <c r="A80" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B80" s="4" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B60" s="4" t="s">
+    <row r="81" spans="1:2">
+      <c r="A81" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B81" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B61" s="4" t="s">
+    <row r="82" spans="1:2">
+      <c r="A82" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B82" s="4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B62" s="4" t="s">
+    <row r="83" spans="1:2">
+      <c r="A83" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B83" s="4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B63" s="4" t="s">
+    <row r="84" spans="1:2">
+      <c r="A84" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B84" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B64" s="4" t="s">
+    <row r="85" spans="1:2">
+      <c r="A85" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B85" s="4" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B65" s="4" t="s">
+    <row r="86" spans="1:2">
+      <c r="A86" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B86" s="4" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B66" s="4" t="s">
+    <row r="87" spans="1:2" ht="27.75">
+      <c r="A87" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B87" s="4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B67" s="4" t="s">
+    <row r="88" spans="1:2">
+      <c r="A88" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B88" s="4" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B68" s="4" t="s">
+    <row r="89" spans="1:2">
+      <c r="A89" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B89" s="4" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B69" s="4" t="s">
+    <row r="90" spans="1:2">
+      <c r="A90" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B90" s="4" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B70" s="4" t="s">
+    <row r="91" spans="1:2">
+      <c r="A91" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B91" s="4" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B71" s="4" t="s">
+    <row r="92" spans="1:2">
+      <c r="A92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B92" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B72" s="4" t="s">
+    <row r="93" spans="1:2">
+      <c r="A93" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B93" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B73" s="4" t="s">
+    <row r="94" spans="1:2">
+      <c r="A94" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B94" s="4" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B74" s="4" t="s">
+    <row r="95" spans="1:2">
+      <c r="A95" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B95" s="4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B75" s="4" t="s">
+    <row r="96" spans="1:2">
+      <c r="A96" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B96" s="4" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B76" s="4" t="s">
+    <row r="97" spans="1:2">
+      <c r="A97" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B97" s="4" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B77" s="4" t="s">
+    <row r="98" spans="1:2">
+      <c r="A98" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B98" s="4" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B78" s="4" t="s">
+    <row r="99" spans="1:2">
+      <c r="A99" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B99" s="4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B79" s="4" t="s">
+    <row r="100" spans="1:2">
+      <c r="A100" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B100" s="4" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B80" s="4" t="s">
+    <row r="101" spans="1:2">
+      <c r="A101" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B101" s="4" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B81" s="4" t="s">
+    <row r="102" spans="1:2">
+      <c r="A102" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B102" s="4" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B82" s="4" t="s">
+    <row r="103" spans="1:2">
+      <c r="A103" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B103" s="4" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B83" s="4" t="s">
+    <row r="104" spans="1:2">
+      <c r="A104" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B104" s="4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B84" s="4" t="s">
+    <row r="105" spans="1:2">
+      <c r="A105" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B107" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B85" s="4" t="s">
+    <row r="108" spans="1:2">
+      <c r="A108" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B108" s="4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B86" s="4" t="s">
+    <row r="109" spans="1:2">
+      <c r="A109" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B109" s="4" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B87" s="4" t="s">
+    <row r="110" spans="1:2">
+      <c r="A110" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B110" s="4" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B88" s="4" t="s">
+    <row r="111" spans="1:2" ht="27.75">
+      <c r="A111" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B111" s="4" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B89" s="4" t="s">
+    <row r="112" spans="1:2">
+      <c r="A112" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B112" s="4" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B90" s="4" t="s">
+    <row r="113" spans="1:2">
+      <c r="A113" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B113" s="4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B91" s="4" t="s">
+    <row r="114" spans="1:2">
+      <c r="A114" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B116" s="4" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B92" s="4" t="s">
+    <row r="117" spans="1:2">
+      <c r="A117" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B117" s="4" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B93" s="4" t="s">
+    <row r="118" spans="1:2">
+      <c r="A118" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B118" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B94" s="4" t="s">
+    <row r="119" spans="1:2">
+      <c r="A119" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B120" s="4" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B95" s="4" t="s">
+    <row r="121" spans="1:2">
+      <c r="A121" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B121" s="4" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B96" s="4" t="s">
+    <row r="122" spans="1:2">
+      <c r="A122" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B122" s="4" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B97" s="4" t="s">
+    <row r="123" spans="1:2">
+      <c r="A123" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B123" s="4" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B98" s="4" t="s">
+    <row r="124" spans="1:2">
+      <c r="A124" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="27.75">
+      <c r="A125" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B125" s="4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B99" s="4" t="s">
+    <row r="126" spans="1:2" ht="27.75">
+      <c r="A126" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B126" s="4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B100" s="4" t="s">
+    <row r="127" spans="1:2" ht="27.75">
+      <c r="A127" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B127" s="4" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
-      <c r="A101" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B101" s="4" t="s">
+    <row r="128" spans="1:2">
+      <c r="A128" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B128" s="4" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B102" s="4" t="s">
+    <row r="129" spans="1:2">
+      <c r="A129" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B130" s="4" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B103" s="4" t="s">
+    <row r="131" spans="1:2">
+      <c r="A131" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B131" s="4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
-      <c r="A104" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B104" s="4" t="s">
+    <row r="132" spans="1:2">
+      <c r="A132" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B132" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
-      <c r="A105" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B105" s="4" t="s">
+    <row r="133" spans="1:2">
+      <c r="A133" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B133" s="4" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B106" s="4" t="s">
+    <row r="134" spans="1:2">
+      <c r="A134" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B134" s="4" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
-      <c r="A107" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B107" s="4" t="s">
+    <row r="135" spans="1:2">
+      <c r="A135" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B135" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B108" s="4" t="s">
+    <row r="136" spans="1:2">
+      <c r="A136" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B136" s="4" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
-      <c r="A109" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B109" s="4" t="s">
+    <row r="137" spans="1:2">
+      <c r="A137" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B137" s="4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
-      <c r="A110" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B110" s="4" t="s">
+    <row r="138" spans="1:2">
+      <c r="A138" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B138" s="4" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
-      <c r="A111" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B111" s="4" t="s">
+    <row r="139" spans="1:2" ht="16.5" customHeight="1">
+      <c r="A139" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="68.25">
+      <c r="A140" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B141" s="4" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
-      <c r="A112" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B112" s="4" t="s">
+    <row r="142" spans="1:2">
+      <c r="A142" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B142" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
-      <c r="A113" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B113" s="4" t="s">
+    <row r="143" spans="1:2">
+      <c r="A143" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B143" s="4" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
-      <c r="A114" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B114" s="4" t="s">
+    <row r="144" spans="1:2" ht="27.75">
+      <c r="A144" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B144" s="4" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
-      <c r="A115" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B115" s="4" t="s">
+    <row r="145" spans="1:2">
+      <c r="A145" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B145" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
-      <c r="A116" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B116" s="4" t="s">
+    <row r="146" spans="1:2" ht="28.5">
+      <c r="A146" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B146" s="4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
-      <c r="A117" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B117" s="4" t="s">
+    <row r="147" spans="1:2">
+      <c r="A147" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B147" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
-      <c r="A118" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B118" s="4" t="s">
+    <row r="148" spans="1:2">
+      <c r="A148" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B148" s="4" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
-      <c r="A119" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B119" s="4" t="s">
+    <row r="149" spans="1:2" ht="41.25">
+      <c r="A149" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B150" s="4" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
-      <c r="A120" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="A121" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
-      <c r="A122" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
-      <c r="A123" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B123" s="4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
-      <c r="A124" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B124" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
-      <c r="A125" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B125" s="4" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
-      <c r="A126" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B126" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
-      <c r="A127" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B127" s="4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
-      <c r="A128" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B128" s="4" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2">
-      <c r="A129" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B129" s="4" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2">
-      <c r="A130" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2">
-      <c r="A131" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B131" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2">
-      <c r="A132" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2">
-      <c r="A133" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2">
-      <c r="A134" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B134" s="4" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2">
-      <c r="A135" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B135" s="4" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2">
-      <c r="A136" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B136" s="4" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2">
-      <c r="A137" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B137" s="4" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2">
-      <c r="A138" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B138" s="4" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A139" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B139" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2">
-      <c r="A140" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2">
-      <c r="A141" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2">
-      <c r="A142" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2">
-      <c r="A143" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B143" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2">
-      <c r="A144" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B144" s="4" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2">
-      <c r="A145" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2">
-      <c r="A146" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B146" s="4" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2">
-      <c r="A147" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B147" s="4" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2">
-      <c r="A148" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B148" s="4" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2">
-      <c r="A149" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B149" s="4" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2">
-      <c r="A150" s="1" t="s">
+    <row r="151" spans="1:2" ht="27.75">
+      <c r="A151" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="B150" s="4" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2">
-      <c r="A151" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="B151" s="4" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="152" spans="1:2">
-      <c r="A152" s="1" t="s">
-        <v>135</v>
+      <c r="A152" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>304</v>
+        <v>272</v>
       </c>
     </row>
     <row r="153" spans="1:2">
-      <c r="A153" s="1" t="s">
+      <c r="A153" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B153" s="4" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2">
-      <c r="A154" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="B154" s="4" t="s">
-        <v>306</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>